<commit_message>
Header done, Badges added
</commit_message>
<xml_diff>
--- a/api_reference.xlsx
+++ b/api_reference.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,295 +453,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>#### Get all products with latest price history and send email notification
+          <t>#### Get all products
 ```http
-GET /api/products
+  GET /api/products
 ```
 | Parameter | Type     | Description                |
 | :-------- | :------- | :------------------------- |
-| `api_key` | `string` | **Required**. Your API key |
-Note: There is only one parameter, which is the API key required for authentication. The rest of the parameters are internally handled by the function, such as product URL and email notification type.</t>
+| None      |          |                             |
+There are no additional parameters or endpoints in this code snippet. The API endpoint `/api/products` uses the `GET` HTTP method to fetch all products from the database.
+Note: This code snippet does not contain any other API methods like POST, PUT, DELETE etc.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Daraz_Scraper\app\products\[id]\page.tsx</t>
+          <t>Daraz_Scraper\app\api\cron\route.ts</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>#### Get product details by ID
+          <t>#### Get all products
 ```http
-GET /api/products/{id}
+  GET /api/products
 ```
 | Parameter | Type     | Description                |
 | :-------- | :------- | :------------------------- |
-| `id`       | `string` | **Required**. The ID of the product to retrieve |
-The API endpoint is `/api/products/{id}`, where `{id}` is a required parameter of type `string`. This endpoint returns the details of a specific product by its ID.
-Note: There are no other parameters or query strings in this API endpoint. The endpoint only expects the `id` parameter to be passed as part of the URL.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\components\Modal.tsx</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>#### Add user email to product
-```http
-  POST /api/products/{productId}/add-email
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `email`   | `string` | **Required**. User's email address |
-| `productId` | `string` | **Path parameter**. The ID of the product to add email to |
-Note: There is only one API endpoint in this code snippet, which is used to add a user's email address to a specific product. It uses a POST request and expects two parameters: `email` and `productId`.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\mongoose.ts</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>#### Connect to MongoDB
-```http
-POST /api/db/connect
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `MONGODB_URI`| `string`| **Required**. Your MongoDB connection string |
-| `strictQuery`| `boolean`| **Optional**. Enable strict query mode |</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\action\index.ts</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>#### Product Management API
-```http
-POST /api/products/scrapeAndStoreProduct
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `productUrl` | `string` | **Required**. URL of the product to scrape and store |
-#### Get Product by ID API
-```http
-GET /api/products/getProductById/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to retrieve |
-| `api_key` | `string` | **Optional**. Your API key |
-#### Get All Products API
-```http
-GET /api/products/getAllProducts
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `api_key` | `string` | **Optional**. Your API key |
-| `limit`   | `integer`| **Optional**. Limit the number of products |
-#### Get Similar Products API
-```http
-GET /api/products/getSimilarProducts/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to retrieve similar products for |
-#### Add User Email to Product API
-```http
-POST /api/products/addUserEmailToProduct/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to add user email to |
-| `userEmail`   | `string` | **Required**. Email address of the user to add |</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\scrapper\index.ts</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>#### Scraping Daraz Products
-```http
-GET /api/daraz/scrape
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `url`     | `string` | **Required**. The URL of the product to scrape |
-| `username`| `string` | **Required**. Your Bright Data username |
-| `password`| `string` | **Required**. Your Bright Data password |
-| `port`    | `integer`| **Required**. The port number for the Bright Data proxy (default: 22225) |
-| `session_id`| `integer` | **Required**. A random session ID |
-Note: This API reference is specific to the scrapingDarazProduct function in the provided code snippet.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\app\api\cron\route.ts</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>#### Get all products with latest price history and send email notification
-```http
-GET /api/products
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `api_key` | `string` | **Required**. Your API key |
-Note: There is only one parameter, which is the API key required for authentication. The rest of the parameters are internally handled by the function, such as product URL and email notification type.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\app\products\[id]\page.tsx</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>#### Get product details by ID
-```http
-GET /api/products/{id}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `id`       | `string` | **Required**. The ID of the product to retrieve |
-The API endpoint is `/api/products/{id}`, where `{id}` is a required parameter of type `string`. This endpoint returns the details of a specific product by its ID.
-Note: There are no other parameters or query strings in this API endpoint. The endpoint only expects the `id` parameter to be passed as part of the URL.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\components\Modal.tsx</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>#### Add user email to product
-```http
-  POST /api/products/{productId}/add-email
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `email`   | `string` | **Required**. User's email address |
-| `productId` | `string` | **Path parameter**. The ID of the product to add email to |
-Note: There is only one API endpoint in this code snippet, which is used to add a user's email address to a specific product. It uses a POST request and expects two parameters: `email` and `productId`.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\mongoose.ts</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>#### Connect to MongoDB
-```http
-POST /api/db/connect
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `MONGODB_URI`| `string`| **Required**. Your MongoDB connection string |
-| `strictQuery`| `boolean`| **Optional**. Enable strict query mode |</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\action\index.ts</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>#### Product Management API
-```http
-POST /api/products/scrapeAndStoreProduct
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `productUrl` | `string` | **Required**. URL of the product to scrape and store |
-#### Get Product by ID API
-```http
-GET /api/products/getProductById/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to retrieve |
-| `api_key` | `string` | **Optional**. Your API key |
-#### Get All Products API
-```http
-GET /api/products/getAllProducts
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `api_key` | `string` | **Optional**. Your API key |
-| `limit`   | `integer`| **Optional**. Limit the number of products |
-#### Get Similar Products API
-```http
-GET /api/products/getSimilarProducts/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to retrieve similar products for |
-#### Add User Email to Product API
-```http
-POST /api/products/addUserEmailToProduct/{productId}
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `{productId}` | `string` | **Path parameter**. ID of the product to add user email to |
-| `userEmail`   | `string` | **Required**. Email address of the user to add |</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Daraz_Scraper\lib\scrapper\index.ts</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>#### Scraping Daraz Products
-```http
-GET /api/daraz/scrape
-```
-| Parameter | Type     | Description                |
-| :-------- | :------- | :------------------------- |
-| `url`     | `string` | **Required**. The URL of the product to scrape |
-| `username`| `string` | **Required**. Your Bright Data username |
-| `password`| `string` | **Required**. Your Bright Data password |
-| `port`    | `integer`| **Required**. The port number for the Bright Data proxy (default: 22225) |
-| `session_id`| `integer` | **Required**. A random session ID |
-Note: This API reference is specific to the scrapingDarazProduct function in the provided code snippet.</t>
+| None      |          |                             |
+There are no additional parameters or endpoints in this code snippet. The API endpoint `/api/products` uses the `GET` HTTP method to fetch all products from the database.
+Note: This code snippet does not contain any other API methods like POST, PUT, DELETE etc.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: cloning location changed to Github_repos
</commit_message>
<xml_diff>
--- a/api_reference.xlsx
+++ b/api_reference.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Daraz_Scraper\app\api\cron\route.ts</t>
+          <t>Github_repos\Daraz_Scraper\app\api\cron\route.ts</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -459,16 +459,32 @@
 ```
 | Parameter | Type     | Description                |
 | :-------- | :------- | :------------------------- |
-| None      |          |                             |
-There are no additional parameters or endpoints in this code snippet. The API endpoint `/api/products` uses the `GET` HTTP method to fetch all products from the database.
-Note: This code snippet does not contain any other API methods like POST, PUT, DELETE etc.</t>
+| None      |          |                            |
+Note: There are no parameters required or optional for this API endpoint. It simply retrieves all products from the database.
+#### Update a product
+```http
+  PUT /api/products/:id
+```
+| Parameter | Type     | Description                |
+| :-------- | :------- | :------------------------- |
+| `id`      | `string` | **Required**. ID of the product to update |
+Note: This endpoint is used to update a specific product in the database, identified by its unique ID.
+#### Send email notification
+```http
+  POST /api/send-email-notification
+```
+| Parameter | Type     | Description                |
+| :-------- | :------- | :------------------------- |
+| None      |          |                            |
+Note: This endpoint sends an email notification to users who have subscribed to updates for a specific product. It does not require any parameters.
+No other API references with HTTP methods were found in the provided code.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Daraz_Scraper\app\api\cron\route.ts</t>
+          <t>Github_repos\Daraz_Scraper\app\api\cron\route.ts</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -479,9 +495,25 @@
 ```
 | Parameter | Type     | Description                |
 | :-------- | :------- | :------------------------- |
-| None      |          |                             |
-There are no additional parameters or endpoints in this code snippet. The API endpoint `/api/products` uses the `GET` HTTP method to fetch all products from the database.
-Note: This code snippet does not contain any other API methods like POST, PUT, DELETE etc.</t>
+| None      |          |                            |
+Note: There are no parameters required or optional for this API endpoint. It simply retrieves all products from the database.
+#### Update a product
+```http
+  PUT /api/products/:id
+```
+| Parameter | Type     | Description                |
+| :-------- | :------- | :------------------------- |
+| `id`      | `string` | **Required**. ID of the product to update |
+Note: This endpoint is used to update a specific product in the database, identified by its unique ID.
+#### Send email notification
+```http
+  POST /api/send-email-notification
+```
+| Parameter | Type     | Description                |
+| :-------- | :------- | :------------------------- |
+| None      |          |                            |
+Note: This endpoint sends an email notification to users who have subscribed to updates for a specific product. It does not require any parameters.
+No other API references with HTTP methods were found in the provided code.</t>
         </is>
       </c>
     </row>

</xml_diff>